<commit_message>
extracted promo and show titles
</commit_message>
<xml_diff>
--- a/docs/Intents.xlsx
+++ b/docs/Intents.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\206534621\Documents\_Code\Alexa-Marketing\docs\"/>
@@ -27,69 +27,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
   <si>
     <t>010 - DigitalPromoIntent</t>
   </si>
   <si>
-    <t>When did {promo} run?</t>
-  </si>
-  <si>
-    <t>promo refers to both on-air and digital promos. Each promo has a promo code</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>hit time, program airing, program information (which program did it run at, promo code), ratings, video link</t>
   </si>
   <si>
-    <t>Where did {promo} run?</t>
-  </si>
-  <si>
-    <t>When and where did {promo} run?</t>
-  </si>
-  <si>
-    <t>What {show} promos are available to run right now?</t>
-  </si>
-  <si>
     <t>Wants to see all length promos</t>
   </si>
   <si>
-    <t>Is the {promo} for {show} available run now?</t>
-  </si>
-  <si>
     <t>Need to get more details on what the question should return</t>
   </si>
   <si>
-    <t>What promos aired for {show} for {date} through {date}</t>
-  </si>
-  <si>
     <t>This is a dashboarding (visual) feature</t>
   </si>
   <si>
-    <t>How much have we spent on music for {show_name}?</t>
-  </si>
-  <si>
     <t>cost collumn needs to be added to VCD</t>
   </si>
   <si>
-    <t>When was the last time promo {video_title} aired?</t>
-  </si>
-  <si>
     <t>What spot has been used most by {show_name}?</t>
-  </si>
-  <si>
-    <t>What ran on air on {date}?</t>
-  </si>
-  <si>
-    <t>Show me all the {length} promos available to run for {show_name}.</t>
-  </si>
-  <si>
-    <t>Give me all promo airings from last night for {show_name}</t>
-  </si>
-  <si>
-    <t>Give me all the promos that aired during {show_name}</t>
   </si>
   <si>
     <t>011 - OnAirPromoIntent</t>
@@ -177,6 +138,42 @@
   </si>
   <si>
     <t>General Notes</t>
+  </si>
+  <si>
+    <t>When did {PromoName} run?</t>
+  </si>
+  <si>
+    <t>Where did {PromoName} run?</t>
+  </si>
+  <si>
+    <t>When and where did {PromoName} run?</t>
+  </si>
+  <si>
+    <t>What {ShowName} promos are available to run right now?</t>
+  </si>
+  <si>
+    <t>Is the {PromoName} for {ShowName} available to run now?</t>
+  </si>
+  <si>
+    <t>What promos aired for {ShowName} from {StartDate} to {EndDate}?</t>
+  </si>
+  <si>
+    <t>How much have we spent on music for {ShowName}?</t>
+  </si>
+  <si>
+    <t>Show me all the {Length} second promos available to run for {ShowName}.</t>
+  </si>
+  <si>
+    <t>When was the last time {PromoName} aired?</t>
+  </si>
+  <si>
+    <t>Give me all promo airings from last night for {ShowName}.</t>
+  </si>
+  <si>
+    <t>What ran on air on {AirDate}?</t>
+  </si>
+  <si>
+    <t>Give me all the promos that aired during {ShowName}.</t>
   </si>
 </sst>
 </file>
@@ -223,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -231,11 +228,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -245,12 +251,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -266,18 +305,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Sheet3"/>
-      <sheetName val="1 - ROLES AND DECISIONS"/>
       <sheetName val="2 - INTENTS"/>
-      <sheetName val="3 - UTTERANCES"/>
-      <sheetName val="DATA POINT REFERENCE"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -552,13 +583,13 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="88.140625" bestFit="1" customWidth="1"/>
@@ -569,13 +600,11 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -583,13 +612,11 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -598,13 +625,11 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -613,13 +638,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -628,13 +653,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -643,13 +668,13 @@
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -658,13 +683,13 @@
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -673,11 +698,11 @@
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -686,11 +711,11 @@
         <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -699,11 +724,11 @@
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -712,11 +737,11 @@
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -725,153 +750,153 @@
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="2"/>
+    <row r="13" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change import script to a single db
</commit_message>
<xml_diff>
--- a/docs/Intents.xlsx
+++ b/docs/Intents.xlsx
@@ -212,12 +212,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -241,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -256,6 +262,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,7 +590,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +606,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C1" s="2"/>
@@ -611,7 +618,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="2"/>
@@ -624,7 +631,7 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="2"/>

</xml_diff>

<commit_message>
fixed issue with session ending. Now the skill can be queried multiple times
</commit_message>
<xml_diff>
--- a/docs/Intents.xlsx
+++ b/docs/Intents.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\_Code\Alexa-Marketing\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\206534621\Documents\_Code\Alexa-Marketing\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
   <si>
     <t>010 - DigitalPromoIntent</t>
   </si>
@@ -86,51 +86,12 @@
     <t>Show me the length of promos for {show_name}.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Dashboarding feature. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Will need more clarification</t>
-    </r>
-  </si>
-  <si>
     <t>Show me the length of promos for {genre}.</t>
   </si>
   <si>
     <t>Give me every promo for {show_name} that ran last week.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Reporting feature. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Will need more clarification about what every promo needs</t>
-    </r>
-  </si>
-  <si>
     <t>What are the rating points for {show_name}?</t>
   </si>
   <si>
@@ -174,12 +135,21 @@
   </si>
   <si>
     <t>Give me all the promos that aired during {ShowName}.</t>
+  </si>
+  <si>
+    <t>Same as last week</t>
+  </si>
+  <si>
+    <t>Same as last night</t>
+  </si>
+  <si>
+    <t>Currently no data for genre.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -212,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,12 +192,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -253,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -269,7 +233,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -320,18 +283,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Sheet3"/>
-      <sheetName val="1 - ROLES AND DECISIONS"/>
       <sheetName val="2 - INTENTS"/>
-      <sheetName val="3 - UTTERANCES"/>
-      <sheetName val="DATA POINT REFERENCE"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -606,7 +561,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -635,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
@@ -648,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
@@ -661,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
@@ -675,8 +630,8 @@
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>30</v>
+      <c r="B5" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
@@ -691,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -706,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -721,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
@@ -747,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -760,7 +715,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
@@ -773,9 +728,11 @@
         <v>0</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>1</v>
       </c>
@@ -785,8 +742,8 @@
       <c r="A13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>37</v>
+      <c r="B13" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6" t="s">
@@ -858,12 +815,10 @@
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="C18" s="3"/>
       <c r="D18" s="2" t="s">
         <v>1</v>
       </c>
@@ -874,10 +829,10 @@
         <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>1</v>
@@ -888,11 +843,11 @@
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>21</v>
+      <c r="B20" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>1</v>
@@ -904,10 +859,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>1</v>
@@ -916,7 +871,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>2</v>
@@ -930,7 +885,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'C:\Users\Nick\Documents\_Code\Alexa-Marketing\docs\[Marketing - AFFINITY_ALEXA DECISIONS AND INTENTS TEMPLATE.xlsx]2 - INTENTS'!#REF!</xm:f>
+            <xm:f>'[1]2 - INTENTS'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>A1:A21</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
Added comments to index.js
</commit_message>
<xml_diff>
--- a/docs/Intents.xlsx
+++ b/docs/Intents.xlsx
@@ -27,15 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
-  <si>
-    <t>010 - DigitalPromoIntent</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>What spot has been used most by {show_name}?</t>
-  </si>
-  <si>
-    <t>011 - OnAirPromoIntent</t>
   </si>
   <si>
     <t>What are the {rating type} ratings for {show_name}?</t>
@@ -197,6 +191,15 @@
   </si>
   <si>
     <t>Show me all the 30 second promos available to run for World of Dance</t>
+  </si>
+  <si>
+    <t>ShowLengthIntent</t>
+  </si>
+  <si>
+    <t>OnAirPromoIntent</t>
+  </si>
+  <si>
+    <t>DigitalPromoIntent</t>
   </si>
 </sst>
 </file>
@@ -287,9 +290,6 @@
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -305,33 +305,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,329 +657,313 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="88.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="13" t="s">
+    </row>
+    <row r="2" spans="1:5" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="E2" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="C8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="E9" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup scale="93" orientation="landscape" verticalDpi="0" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'[1]2 - INTENTS'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A20</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>